<commit_message>
add DQC_0013 elements V2 revised
</commit_message>
<xml_diff>
--- a/meetings/apr_2016/DQC_0013_ListOfElements_V2.xlsx.xlsx
+++ b/meetings/apr_2016/DQC_0013_ListOfElements_V2.xlsx.xlsx
@@ -62,13 +62,13 @@
                                         IncomeLossFromContinuingOperationsBeforeIncomeTaxesExtraordinaryItemsNoncontrollingInterest.value
                                 else
                                         if(exists(IncomeLossFromContinuingOperationsBeforeIncomeTaxesMinorityInterestAndIncomeLossFromEquityMethodInvestments.value))
-                                        IncomeLossFromContinuingOperationsBeforeIncomeTaxesMinorityInterestAndIncomeLossFromEquityMethodInvestments.value - 
+                                        IncomeLossFromContinuingOperationsBeforeIncomeTaxesMinorityInterestAndIncomeLossFromEquityMethodInvestments.value + 
                                         IncomeLossFromEquityMethodInvestments.value
                                         else
                                                 if        (exists(IncomeLossFromContinuingOperationsBeforeIncomeTaxesDomestic.value) or 
                                                           exists(IncomeLossFromContinuingOperationsBeforeIncomeTaxesForeign.value))
                                                         IncomeLossFromContinuingOperationsBeforeIncomeTaxesDomestic.value +
-                                                        IncomeLossFromContinuingOperationsBeforeIncomeTaxesForeign.value -
+                                                        IncomeLossFromContinuingOperationsBeforeIncomeTaxesForeign.value +
                                                         IncomeLossFromEquityMethodInvestments.value
                                                 else
                                                        0)</t>

</xml_diff>